<commit_message>
Tested the terminal and made necessary changes
</commit_message>
<xml_diff>
--- a/PacificLB/Test.xlsx
+++ b/PacificLB/Test.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\PortTerminalScraping\PacificLB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -134,224 +141,223 @@
     <t>DENU2012180</t>
   </si>
   <si>
+    <t>COSU6198972540</t>
+  </si>
+  <si>
+    <t>7075414135</t>
+  </si>
+  <si>
+    <t>060E</t>
+  </si>
+  <si>
+    <t>CBHU4321947</t>
+  </si>
+  <si>
+    <t>2106465680</t>
+  </si>
+  <si>
+    <t>7075412661</t>
+  </si>
+  <si>
+    <t>DJLAXA4123414</t>
+  </si>
+  <si>
+    <t>OOCU7690470</t>
+  </si>
+  <si>
+    <t>SGN900499500</t>
+  </si>
+  <si>
+    <t>7075408528</t>
+  </si>
+  <si>
+    <t>DJLAXA4129694</t>
+  </si>
+  <si>
+    <t>00023</t>
+  </si>
+  <si>
+    <t>PCIU1422504</t>
+  </si>
+  <si>
+    <t>6205087532</t>
+  </si>
+  <si>
+    <t>7075414650</t>
+  </si>
+  <si>
+    <t>CSLU1531853</t>
+  </si>
+  <si>
+    <t>6202944660</t>
+  </si>
+  <si>
+    <t>7075415546</t>
+  </si>
+  <si>
+    <t>CSNU4086954</t>
+  </si>
+  <si>
+    <t>CBHU6386320</t>
+  </si>
+  <si>
+    <t>CCLU4611268</t>
+  </si>
+  <si>
+    <t>FSCU5101409</t>
+  </si>
+  <si>
+    <t>CCLU5224237</t>
+  </si>
+  <si>
+    <t>CCLU5296345</t>
+  </si>
+  <si>
+    <t>6205089193</t>
+  </si>
+  <si>
+    <t>7075414546</t>
+  </si>
+  <si>
+    <t>FCIU9772258</t>
+  </si>
+  <si>
+    <t>7075412665</t>
+  </si>
+  <si>
+    <t>DJLAXA4123430</t>
+  </si>
+  <si>
+    <t>TCLU1480849</t>
+  </si>
+  <si>
+    <t>7075412664</t>
+  </si>
+  <si>
+    <t>DJLAXA4123422</t>
+  </si>
+  <si>
+    <t>OOCU7826361</t>
+  </si>
+  <si>
+    <t>7075412663</t>
+  </si>
+  <si>
+    <t>DJLAXA4123419</t>
+  </si>
+  <si>
+    <t>OOLU9600451</t>
+  </si>
+  <si>
+    <t>HUPE90049700</t>
+  </si>
+  <si>
+    <t>7075412761</t>
+  </si>
+  <si>
+    <t>PCIU9153612</t>
+  </si>
+  <si>
+    <t>SEGU6133782</t>
+  </si>
+  <si>
+    <t>PCIU8646492</t>
+  </si>
+  <si>
+    <t>CKBH80037500</t>
+  </si>
+  <si>
+    <t>7075391630</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>PCIU9152323</t>
+  </si>
+  <si>
+    <t>PCIU8292254</t>
+  </si>
+  <si>
+    <t>6192866750</t>
+  </si>
+  <si>
+    <t>7075405220</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>CSNU7127002</t>
+  </si>
+  <si>
+    <t>CBHU8648326</t>
+  </si>
+  <si>
+    <t>SGN900510600</t>
+  </si>
+  <si>
+    <t>7075408655</t>
+  </si>
+  <si>
+    <t>DJLAXA4129584</t>
+  </si>
+  <si>
+    <t>TGHU9679522</t>
+  </si>
+  <si>
+    <t>7075412662</t>
+  </si>
+  <si>
+    <t>DJLAXA4123417</t>
+  </si>
+  <si>
+    <t>OOCU7455810</t>
+  </si>
+  <si>
+    <t>SGN900428600</t>
+  </si>
+  <si>
+    <t>7075407634</t>
+  </si>
+  <si>
+    <t>DJLAXA4123378</t>
+  </si>
+  <si>
+    <t>PCIU0061264</t>
+  </si>
+  <si>
+    <t>7075412666</t>
+  </si>
+  <si>
+    <t>DJLAXA4123415</t>
+  </si>
+  <si>
+    <t>OOCU7715331</t>
+  </si>
+  <si>
+    <t>SZX901067400</t>
+  </si>
+  <si>
+    <t>7075414773</t>
+  </si>
+  <si>
+    <t>PCIU1541099</t>
+  </si>
+  <si>
+    <t>DENU2012220</t>
+  </si>
+  <si>
     <t>DENU2012241</t>
-  </si>
-  <si>
-    <t>DENU2012220</t>
-  </si>
-  <si>
-    <t>PCIU1541099</t>
-  </si>
-  <si>
-    <t>00023</t>
-  </si>
-  <si>
-    <t>7075414773</t>
-  </si>
-  <si>
-    <t>SZX901067400</t>
-  </si>
-  <si>
-    <t>OOCU7715331</t>
-  </si>
-  <si>
-    <t>DJLAXA4123415</t>
-  </si>
-  <si>
-    <t>7075412666</t>
-  </si>
-  <si>
-    <t>2106465680</t>
-  </si>
-  <si>
-    <t>PCIU0061264</t>
-  </si>
-  <si>
-    <t>DJLAXA4123378</t>
-  </si>
-  <si>
-    <t>7075407634</t>
-  </si>
-  <si>
-    <t>SGN900428600</t>
-  </si>
-  <si>
-    <t>OOCU7455810</t>
-  </si>
-  <si>
-    <t>DJLAXA4123417</t>
-  </si>
-  <si>
-    <t>7075412662</t>
-  </si>
-  <si>
-    <t>TGHU9679522</t>
-  </si>
-  <si>
-    <t>DJLAXA4129584</t>
-  </si>
-  <si>
-    <t>7075408655</t>
-  </si>
-  <si>
-    <t>SGN900510600</t>
-  </si>
-  <si>
-    <t>CBHU8648326</t>
-  </si>
-  <si>
-    <t>060</t>
-  </si>
-  <si>
-    <t>7075405220</t>
-  </si>
-  <si>
-    <t>6192866750</t>
-  </si>
-  <si>
-    <t>CSNU7127002</t>
-  </si>
-  <si>
-    <t>PCIU8292254</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>7075391630</t>
-  </si>
-  <si>
-    <t>CKBH80037500</t>
-  </si>
-  <si>
-    <t>PCIU9152323</t>
-  </si>
-  <si>
-    <t>PCIU8646492</t>
-  </si>
-  <si>
-    <t>7075412761</t>
-  </si>
-  <si>
-    <t>HUPE90049700</t>
-  </si>
-  <si>
-    <t>SEGU6133782</t>
-  </si>
-  <si>
-    <t>PCIU9153612</t>
-  </si>
-  <si>
-    <t>OOLU9600451</t>
-  </si>
-  <si>
-    <t>DJLAXA4123419</t>
-  </si>
-  <si>
-    <t>7075412663</t>
-  </si>
-  <si>
-    <t>OOCU7826361</t>
-  </si>
-  <si>
-    <t>DJLAXA4123422</t>
-  </si>
-  <si>
-    <t>7075412664</t>
-  </si>
-  <si>
-    <t>TCLU1480849</t>
-  </si>
-  <si>
-    <t>DJLAXA4123430</t>
-  </si>
-  <si>
-    <t>7075412665</t>
-  </si>
-  <si>
-    <t>FCIU9772258</t>
-  </si>
-  <si>
-    <t>7075414546</t>
-  </si>
-  <si>
-    <t>6205089193</t>
-  </si>
-  <si>
-    <t>CCLU5296345</t>
-  </si>
-  <si>
-    <t>7075415546</t>
-  </si>
-  <si>
-    <t>6202944660</t>
-  </si>
-  <si>
-    <t>CCLU5224237</t>
-  </si>
-  <si>
-    <t>FSCU5101409</t>
-  </si>
-  <si>
-    <t>CCLU4611268</t>
-  </si>
-  <si>
-    <t>CBHU6386320</t>
-  </si>
-  <si>
-    <t>CSNU4086954</t>
-  </si>
-  <si>
-    <t>CSLU1531853</t>
-  </si>
-  <si>
-    <t>7075414650</t>
-  </si>
-  <si>
-    <t>6205087532</t>
-  </si>
-  <si>
-    <t>PCIU1422504</t>
-  </si>
-  <si>
-    <t>DJLAXA4129694</t>
-  </si>
-  <si>
-    <t>7075408528</t>
-  </si>
-  <si>
-    <t>SGN900499500</t>
-  </si>
-  <si>
-    <t>OOCU7690470</t>
-  </si>
-  <si>
-    <t>DJLAXA4123414</t>
-  </si>
-  <si>
-    <t>7075412661</t>
-  </si>
-  <si>
-    <t>CBHU4321947</t>
-  </si>
-  <si>
-    <t>060E</t>
-  </si>
-  <si>
-    <t>7075414135</t>
-  </si>
-  <si>
-    <t>COSU6198972540</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -363,7 +369,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -381,18 +387,294 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -432,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -452,7 +734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -472,7 +754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -492,7 +774,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -512,7 +794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -532,7 +814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -552,7 +834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -572,7 +854,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -592,9 +874,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -612,9 +894,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -632,29 +914,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -663,38 +945,38 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -703,118 +985,118 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -823,18 +1105,18 @@
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -843,18 +1125,18 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
@@ -863,18 +1145,18 @@
         <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -883,18 +1165,18 @@
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
@@ -903,18 +1185,18 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -923,38 +1205,38 @@
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -963,18 +1245,18 @@
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -983,18 +1265,18 @@
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
@@ -1003,18 +1285,18 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
@@ -1023,18 +1305,18 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
         <v>29</v>
@@ -1043,18 +1325,18 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -1063,58 +1345,58 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
@@ -1123,36 +1405,36 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="F37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="D38" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>